<commit_message>
Células Vazias e Fonte de Dados
</commit_message>
<xml_diff>
--- a/5-FuncoesMercadoTrabalho/09. Função E - Duas Condições - Material(1).xlsx
+++ b/5-FuncoesMercadoTrabalho/09. Função E - Duas Condições - Material(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\5-FuncoesMercadoTrabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66267ADE-22E0-44C4-99BE-E6D47E3500D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732F432B-5039-4ADE-B1AB-2FBCFBCAAA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="957" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
   </bookViews>
@@ -34,6 +34,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -3086,6 +3089,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3122,7 +3126,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Cancel 14" xfId="3" xr:uid="{CBF31453-4DDC-45BF-AC7E-30D18DBD75F7}"/>
@@ -3443,7 +3446,7 @@
   <dimension ref="A1:M1999"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3528,13 +3531,13 @@
         <f t="shared" ref="G3:G66" si="1">IF(AND(B3 &lt; DATE(2010,12,31), C3 = "Concurso", D3 = "RJ"), "Sim", "Não")</f>
         <v>Não</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="28" t="s">
         <v>884</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -3678,13 +3681,13 @@
         <f t="shared" si="1"/>
         <v>Não</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="25" t="s">
         <v>885</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="27"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -3837,7 +3840,7 @@
         <f t="shared" si="1"/>
         <v>Não</v>
       </c>
-      <c r="J13" s="36">
+      <c r="J13" s="24">
         <v>40543</v>
       </c>
     </row>
@@ -36362,13 +36365,13 @@
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="31" t="s">
         <v>882</v>
       </c>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -36482,13 +36485,13 @@
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="15"/>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="34" t="s">
         <v>883</v>
       </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="36"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">

</xml_diff>